<commit_message>
Conditionally format with color scales
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="F200" sqref="F200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G180" sqref="G180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4062,6 +4062,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E200">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Paste values to eliminate formula
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -446,7 +446,7 @@
   <dimension ref="A1:E203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G180" sqref="G180"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +482,6 @@
         <v>0.5</v>
       </c>
       <c r="E2" s="6">
-        <f>C2*D2</f>
         <v>2</v>
       </c>
     </row>
@@ -500,7 +499,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E66" si="0">C3*D3</f>
         <v>2</v>
       </c>
     </row>
@@ -518,7 +516,6 @@
         <v>0.8</v>
       </c>
       <c r="E4" s="6">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -536,7 +533,6 @@
         <v>0.25</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -554,7 +550,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -572,7 +567,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -590,7 +584,6 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -608,7 +601,6 @@
         <v>0.8</v>
       </c>
       <c r="E9" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -626,7 +618,6 @@
         <v>0.75</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -644,7 +635,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -662,7 +652,6 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -680,7 +669,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -698,7 +686,6 @@
         <v>0.5</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -716,7 +703,6 @@
         <v>0.5</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -734,7 +720,6 @@
         <v>0.5</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -752,7 +737,6 @@
         <v>0.25</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -770,7 +754,6 @@
         <v>0.5</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -788,7 +771,6 @@
         <v>0.8</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -806,7 +788,6 @@
         <v>0.5</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -824,7 +805,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -842,7 +822,6 @@
         <v>0.5</v>
       </c>
       <c r="E22" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -860,7 +839,6 @@
         <v>0.8</v>
       </c>
       <c r="E23" s="6">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -878,7 +856,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E24" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -896,7 +873,6 @@
         <v>0.5</v>
       </c>
       <c r="E25" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -914,7 +890,6 @@
         <v>0.5</v>
       </c>
       <c r="E26" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -932,7 +907,6 @@
         <v>0.5</v>
       </c>
       <c r="E27" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -950,7 +924,6 @@
         <v>0.75</v>
       </c>
       <c r="E28" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -968,7 +941,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E29" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -986,7 +958,6 @@
         <v>0.5</v>
       </c>
       <c r="E30" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1004,7 +975,6 @@
         <v>0.5</v>
       </c>
       <c r="E31" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1022,7 +992,6 @@
         <v>0.8</v>
       </c>
       <c r="E32" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1040,7 +1009,6 @@
         <v>0.5</v>
       </c>
       <c r="E33" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1058,7 +1026,6 @@
         <v>0.5</v>
       </c>
       <c r="E34" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1076,7 +1043,6 @@
         <v>0.5</v>
       </c>
       <c r="E35" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1094,7 +1060,6 @@
         <v>0.5</v>
       </c>
       <c r="E36" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1112,7 +1077,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E37" s="6">
-        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1130,7 +1094,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E38" s="6">
-        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1148,7 +1111,6 @@
         <v>0.8</v>
       </c>
       <c r="E39" s="6">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1166,7 +1128,6 @@
         <v>0.75</v>
       </c>
       <c r="E40" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1184,7 +1145,6 @@
         <v>0.5</v>
       </c>
       <c r="E41" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1202,7 +1162,6 @@
         <v>0.5</v>
       </c>
       <c r="E42" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1220,7 +1179,6 @@
         <v>0.5</v>
       </c>
       <c r="E43" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1238,7 +1196,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E44" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1256,7 +1213,6 @@
         <v>0.75</v>
       </c>
       <c r="E45" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1274,7 +1230,6 @@
         <v>0.25</v>
       </c>
       <c r="E46" s="6">
-        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1292,7 +1247,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E47" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1310,7 +1264,6 @@
         <v>0.5</v>
       </c>
       <c r="E48" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1328,7 +1281,6 @@
         <v>0.5</v>
       </c>
       <c r="E49" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1346,7 +1298,6 @@
         <v>0.5</v>
       </c>
       <c r="E50" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1364,7 +1315,6 @@
         <v>0.8</v>
       </c>
       <c r="E51" s="6">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1382,7 +1332,6 @@
         <v>0.75</v>
       </c>
       <c r="E52" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1400,7 +1349,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E53" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1418,7 +1366,6 @@
         <v>0.8</v>
       </c>
       <c r="E54" s="6">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1436,7 +1383,6 @@
         <v>0.5</v>
       </c>
       <c r="E55" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1454,7 +1400,6 @@
         <v>0.5</v>
       </c>
       <c r="E56" s="6">
-        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1472,7 +1417,6 @@
         <v>0.5</v>
       </c>
       <c r="E57" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1490,7 +1434,6 @@
         <v>0.5</v>
       </c>
       <c r="E58" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1508,7 +1451,6 @@
         <v>0.5</v>
       </c>
       <c r="E59" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1526,7 +1468,6 @@
         <v>0.5</v>
       </c>
       <c r="E60" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1544,7 +1485,6 @@
         <v>0.5</v>
       </c>
       <c r="E61" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1562,7 +1502,6 @@
         <v>0.8</v>
       </c>
       <c r="E62" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1580,7 +1519,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E63" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1598,7 +1536,6 @@
         <v>0.25</v>
       </c>
       <c r="E64" s="6">
-        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1616,7 +1553,6 @@
         <v>0.8</v>
       </c>
       <c r="E65" s="6">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1634,7 +1570,6 @@
         <v>0.5</v>
       </c>
       <c r="E66" s="6">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1652,7 +1587,6 @@
         <v>0.5</v>
       </c>
       <c r="E67" s="6">
-        <f t="shared" ref="E67:E130" si="1">C67*D67</f>
         <v>1.5</v>
       </c>
     </row>
@@ -1670,7 +1604,6 @@
         <v>0.8</v>
       </c>
       <c r="E68" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1688,7 +1621,6 @@
         <v>0.75</v>
       </c>
       <c r="E69" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1706,7 +1638,6 @@
         <v>0.5</v>
       </c>
       <c r="E70" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1724,7 +1655,6 @@
         <v>0.5</v>
       </c>
       <c r="E71" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1742,7 +1672,6 @@
         <v>0.5</v>
       </c>
       <c r="E72" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1760,7 +1689,6 @@
         <v>0.5</v>
       </c>
       <c r="E73" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1778,7 +1706,6 @@
         <v>0.5</v>
       </c>
       <c r="E74" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1796,7 +1723,6 @@
         <v>0.5</v>
       </c>
       <c r="E75" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1814,7 +1740,6 @@
         <v>0.5</v>
       </c>
       <c r="E76" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1832,7 +1757,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E77" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1850,7 +1774,6 @@
         <v>0.25</v>
       </c>
       <c r="E78" s="6">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1868,7 +1791,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E79" s="6">
-        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1886,7 +1808,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E80" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1904,7 +1825,6 @@
         <v>0.5</v>
       </c>
       <c r="E81" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1922,7 +1842,6 @@
         <v>0.8</v>
       </c>
       <c r="E82" s="6">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1940,7 +1859,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E83" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1958,7 +1876,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E84" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1976,7 +1893,6 @@
         <v>0.75</v>
       </c>
       <c r="E85" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1994,7 +1910,6 @@
         <v>0.5</v>
       </c>
       <c r="E86" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2012,7 +1927,6 @@
         <v>0.5</v>
       </c>
       <c r="E87" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2030,7 +1944,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E88" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2048,7 +1961,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E89" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2066,7 +1978,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E90" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2084,7 +1995,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E91" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2102,7 +2012,6 @@
         <v>0.8</v>
       </c>
       <c r="E92" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2120,7 +2029,6 @@
         <v>0.75</v>
       </c>
       <c r="E93" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -2138,7 +2046,6 @@
         <v>0.5</v>
       </c>
       <c r="E94" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2156,7 +2063,6 @@
         <v>0.25</v>
       </c>
       <c r="E95" s="6">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2174,7 +2080,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E96" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2192,7 +2097,6 @@
         <v>0.5</v>
       </c>
       <c r="E97" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2210,7 +2114,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E98" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2228,7 +2131,6 @@
         <v>0.5</v>
       </c>
       <c r="E99" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2246,7 +2148,6 @@
         <v>0.5</v>
       </c>
       <c r="E100" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2264,7 +2165,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E101" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2282,7 +2182,6 @@
         <v>0.5</v>
       </c>
       <c r="E102" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2300,7 +2199,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E103" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2318,7 +2216,6 @@
         <v>0.5</v>
       </c>
       <c r="E104" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2336,7 +2233,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E105" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2354,7 +2250,6 @@
         <v>0.5</v>
       </c>
       <c r="E106" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2372,7 +2267,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E107" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2390,7 +2284,6 @@
         <v>0.8</v>
       </c>
       <c r="E108" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2408,7 +2301,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E109" s="6">
-        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2426,7 +2318,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E110" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2444,7 +2335,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E111" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2462,7 +2352,6 @@
         <v>0.5</v>
       </c>
       <c r="E112" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2480,7 +2369,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E113" s="6">
-        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2498,7 +2386,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E114" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2516,7 +2403,6 @@
         <v>0.8</v>
       </c>
       <c r="E115" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2534,7 +2420,6 @@
         <v>0.25</v>
       </c>
       <c r="E116" s="6">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2552,7 +2437,6 @@
         <v>0.8</v>
       </c>
       <c r="E117" s="6">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -2570,7 +2454,6 @@
         <v>0.8</v>
       </c>
       <c r="E118" s="6">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -2588,7 +2471,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E119" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2606,7 +2488,6 @@
         <v>0.8</v>
       </c>
       <c r="E120" s="6">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -2624,7 +2505,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E121" s="6">
-        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2642,7 +2522,6 @@
         <v>0.5</v>
       </c>
       <c r="E122" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2660,7 +2539,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E123" s="6">
-        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2678,7 +2556,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E124" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2696,7 +2573,6 @@
         <v>0.25</v>
       </c>
       <c r="E125" s="6">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2714,7 +2590,6 @@
         <v>0.25</v>
       </c>
       <c r="E126" s="6">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2732,7 +2607,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E127" s="6">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2750,7 +2624,6 @@
         <v>0.25</v>
       </c>
       <c r="E128" s="6">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2768,7 +2641,6 @@
         <v>0.5</v>
       </c>
       <c r="E129" s="6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2786,7 +2658,6 @@
         <v>0.75</v>
       </c>
       <c r="E130" s="6">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -2804,7 +2675,6 @@
         <v>0.5</v>
       </c>
       <c r="E131" s="6">
-        <f t="shared" ref="E131:E194" si="2">C131*D131</f>
         <v>2</v>
       </c>
     </row>
@@ -2822,7 +2692,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E132" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2840,7 +2709,6 @@
         <v>0.5</v>
       </c>
       <c r="E133" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -2858,7 +2726,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E134" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2876,7 +2743,6 @@
         <v>0.5</v>
       </c>
       <c r="E135" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2894,7 +2760,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E136" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2912,7 +2777,6 @@
         <v>0.75</v>
       </c>
       <c r="E137" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -2930,7 +2794,6 @@
         <v>0.8</v>
       </c>
       <c r="E138" s="6">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -2948,7 +2811,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E139" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2966,7 +2828,6 @@
         <v>0.8</v>
       </c>
       <c r="E140" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -2984,7 +2845,6 @@
         <v>0.25</v>
       </c>
       <c r="E141" s="6">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3002,7 +2862,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E142" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3020,7 +2879,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E143" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3038,7 +2896,6 @@
         <v>0.5</v>
       </c>
       <c r="E144" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3056,7 +2913,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E145" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3074,7 +2930,6 @@
         <v>0.5</v>
       </c>
       <c r="E146" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3092,7 +2947,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E147" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3110,7 +2964,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E148" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3128,7 +2981,6 @@
         <v>0.5</v>
       </c>
       <c r="E149" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3146,7 +2998,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E150" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3164,7 +3015,6 @@
         <v>0.8</v>
       </c>
       <c r="E151" s="6">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3182,7 +3032,6 @@
         <v>0.8</v>
       </c>
       <c r="E152" s="6">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3200,7 +3049,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E153" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3218,7 +3066,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E154" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3236,7 +3083,6 @@
         <v>0.25</v>
       </c>
       <c r="E155" s="6">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3254,7 +3100,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E156" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3272,7 +3117,6 @@
         <v>0.25</v>
       </c>
       <c r="E157" s="6">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3290,7 +3134,6 @@
         <v>0.8</v>
       </c>
       <c r="E158" s="6">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3308,7 +3151,6 @@
         <v>0.8</v>
       </c>
       <c r="E159" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3326,7 +3168,6 @@
         <v>0.5</v>
       </c>
       <c r="E160" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3344,7 +3185,6 @@
         <v>0.5</v>
       </c>
       <c r="E161" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3362,7 +3202,6 @@
         <v>0.5</v>
       </c>
       <c r="E162" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3380,7 +3219,6 @@
         <v>0.5</v>
       </c>
       <c r="E163" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3398,7 +3236,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E164" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3416,7 +3253,6 @@
         <v>0.8</v>
       </c>
       <c r="E165" s="6">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3434,7 +3270,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E166" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3452,7 +3287,6 @@
         <v>0.8</v>
       </c>
       <c r="E167" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3470,7 +3304,6 @@
         <v>0.75</v>
       </c>
       <c r="E168" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3488,7 +3321,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E169" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3506,7 +3338,6 @@
         <v>0.5</v>
       </c>
       <c r="E170" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3524,7 +3355,6 @@
         <v>0.75</v>
       </c>
       <c r="E171" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3542,7 +3372,6 @@
         <v>0.5</v>
       </c>
       <c r="E172" s="6">
-        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -3560,7 +3389,6 @@
         <v>0.5</v>
       </c>
       <c r="E173" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3578,7 +3406,6 @@
         <v>0.5</v>
       </c>
       <c r="E174" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3596,7 +3423,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E175" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3614,7 +3440,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E176" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3632,7 +3457,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E177" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3650,7 +3474,6 @@
         <v>0.5</v>
       </c>
       <c r="E178" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3668,7 +3491,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E179" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3686,7 +3508,6 @@
         <v>0.5</v>
       </c>
       <c r="E180" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3704,7 +3525,6 @@
         <v>0.25</v>
       </c>
       <c r="E181" s="6">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3722,7 +3542,6 @@
         <v>0.5</v>
       </c>
       <c r="E182" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3740,7 +3559,6 @@
         <v>0.8</v>
       </c>
       <c r="E183" s="6">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3758,7 +3576,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E184" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3776,7 +3593,6 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E185" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3794,7 +3610,6 @@
         <v>0.8</v>
       </c>
       <c r="E186" s="6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -3812,7 +3627,6 @@
         <v>0.5</v>
       </c>
       <c r="E187" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3830,7 +3644,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E188" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3848,7 +3661,6 @@
         <v>0.25</v>
       </c>
       <c r="E189" s="6">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3866,7 +3678,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E190" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3884,7 +3695,6 @@
         <v>0.5</v>
       </c>
       <c r="E191" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3902,7 +3712,6 @@
         <v>0.25</v>
       </c>
       <c r="E192" s="6">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3920,7 +3729,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E193" s="6">
-        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3938,7 +3746,6 @@
         <v>0.8</v>
       </c>
       <c r="E194" s="6">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3956,7 +3763,6 @@
         <v>0.5</v>
       </c>
       <c r="E195" s="6">
-        <f t="shared" ref="E195:E200" si="3">C195*D195</f>
         <v>2</v>
       </c>
     </row>
@@ -3974,7 +3780,6 @@
         <v>0.25</v>
       </c>
       <c r="E196" s="6">
-        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3992,7 +3797,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E197" s="6">
-        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
     </row>
@@ -4010,7 +3814,6 @@
         <v>0.75</v>
       </c>
       <c r="E198" s="6">
-        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4028,7 +3831,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E199" s="6">
-        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
     </row>
@@ -4046,7 +3848,6 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E200" s="6">
-        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create clustered column chart and format data series
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,6 +196,926 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calories</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Beer</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bottled Water</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chocolate Bar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Chocolate Dipped Cone</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Gummy Bears</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hamburger</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hot Dog</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ice Cream Sandwich</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Licorice Rope</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Nachos</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pizza</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Popcorn</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Popsicle</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Soda</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>255.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>265.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>560.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2092002624"/>
+        <c:axId val="-2089652448"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2092002624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2089652448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2089652448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2092002624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3900,7 +4820,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4027,5 +4947,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use find and replace all to sub Energy for Calories
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -102,7 +102,7 @@
     <t>Actual Profit</t>
   </si>
   <si>
-    <t>Calories</t>
+    <t>Energy</t>
   </si>
 </sst>
 </file>
@@ -259,7 +259,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Calories</c:v>
+                  <c:v>Energy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4820,7 +4820,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add calories to Sales sheet
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Basketball Game Sales" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="30">
   <si>
     <t>Item</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Actual Profit</t>
+  </si>
+  <si>
+    <t>Calories</t>
   </si>
   <si>
     <t>Energy</t>
@@ -1396,15 +1399,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E203"/>
+  <dimension ref="A1:F203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1420,8 +1423,11 @@
       <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1437,8 +1443,12 @@
       <c r="E2" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <f>VLOOKUP(A2,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1454,8 +1464,12 @@
       <c r="E3" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f>VLOOKUP(A3,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1471,8 +1485,12 @@
       <c r="E4" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f>VLOOKUP(A4,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1488,8 +1506,12 @@
       <c r="E5" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f>VLOOKUP(A5,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1505,8 +1527,12 @@
       <c r="E6" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f>VLOOKUP(A6,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1522,8 +1548,12 @@
       <c r="E7" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f>VLOOKUP(A7,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1539,8 +1569,12 @@
       <c r="E8" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f>VLOOKUP(A8,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1556,8 +1590,12 @@
       <c r="E9" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f>VLOOKUP(A9,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1573,8 +1611,12 @@
       <c r="E10" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f>VLOOKUP(A10,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1590,8 +1632,12 @@
       <c r="E11" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f>VLOOKUP(A11,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1607,8 +1653,12 @@
       <c r="E12" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f>VLOOKUP(A12,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1624,8 +1674,12 @@
       <c r="E13" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f>VLOOKUP(A13,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1641,8 +1695,12 @@
       <c r="E14" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f>VLOOKUP(A14,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1658,8 +1716,12 @@
       <c r="E15" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <f>VLOOKUP(A15,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1675,8 +1737,12 @@
       <c r="E16" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f>VLOOKUP(A16,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1692,8 +1758,12 @@
       <c r="E17" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f>VLOOKUP(A17,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1709,8 +1779,12 @@
       <c r="E18" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <f>VLOOKUP(A18,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1726,8 +1800,12 @@
       <c r="E19" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f>VLOOKUP(A19,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1743,8 +1821,12 @@
       <c r="E20" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f>VLOOKUP(A20,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1760,8 +1842,12 @@
       <c r="E21" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f>VLOOKUP(A21,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1777,8 +1863,12 @@
       <c r="E22" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <f>VLOOKUP(A22,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1794,8 +1884,12 @@
       <c r="E23" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <f>VLOOKUP(A23,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1811,8 +1905,12 @@
       <c r="E24" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <f>VLOOKUP(A24,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1828,8 +1926,12 @@
       <c r="E25" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <f>VLOOKUP(A25,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1845,8 +1947,12 @@
       <c r="E26" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <f>VLOOKUP(A26,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1862,8 +1968,12 @@
       <c r="E27" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <f>VLOOKUP(A27,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1879,8 +1989,12 @@
       <c r="E28" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <f>VLOOKUP(A28,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1896,8 +2010,12 @@
       <c r="E29" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <f>VLOOKUP(A29,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1913,8 +2031,12 @@
       <c r="E30" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <f>VLOOKUP(A30,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1930,8 +2052,12 @@
       <c r="E31" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <f>VLOOKUP(A31,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1947,8 +2073,12 @@
       <c r="E32" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <f>VLOOKUP(A32,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1964,8 +2094,12 @@
       <c r="E33" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <f>VLOOKUP(A33,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1981,8 +2115,12 @@
       <c r="E34" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <f>VLOOKUP(A34,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1998,8 +2136,12 @@
       <c r="E35" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <f>VLOOKUP(A35,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -2015,8 +2157,12 @@
       <c r="E36" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <f>VLOOKUP(A36,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2032,8 +2178,12 @@
       <c r="E37" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <f>VLOOKUP(A37,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2049,8 +2199,12 @@
       <c r="E38" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <f>VLOOKUP(A38,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2066,8 +2220,12 @@
       <c r="E39" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <f>VLOOKUP(A39,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2083,8 +2241,12 @@
       <c r="E40" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <f>VLOOKUP(A40,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2100,8 +2262,12 @@
       <c r="E41" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <f>VLOOKUP(A41,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -2117,8 +2283,12 @@
       <c r="E42" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <f>VLOOKUP(A42,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -2134,8 +2304,12 @@
       <c r="E43" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <f>VLOOKUP(A43,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2151,8 +2325,12 @@
       <c r="E44" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <f>VLOOKUP(A44,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -2168,8 +2346,12 @@
       <c r="E45" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <f>VLOOKUP(A45,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2185,8 +2367,12 @@
       <c r="E46" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <f>VLOOKUP(A46,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -2202,8 +2388,12 @@
       <c r="E47" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <f>VLOOKUP(A47,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2219,8 +2409,12 @@
       <c r="E48" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <f>VLOOKUP(A48,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -2236,8 +2430,12 @@
       <c r="E49" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <f>VLOOKUP(A49,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -2253,8 +2451,12 @@
       <c r="E50" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <f>VLOOKUP(A50,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2270,8 +2472,12 @@
       <c r="E51" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <f>VLOOKUP(A51,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2287,8 +2493,12 @@
       <c r="E52" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <f>VLOOKUP(A52,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -2304,8 +2514,12 @@
       <c r="E53" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <f>VLOOKUP(A53,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2321,8 +2535,12 @@
       <c r="E54" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <f>VLOOKUP(A54,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -2338,8 +2556,12 @@
       <c r="E55" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <f>VLOOKUP(A55,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2355,8 +2577,12 @@
       <c r="E56" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <f>VLOOKUP(A56,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -2372,8 +2598,12 @@
       <c r="E57" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <f>VLOOKUP(A57,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -2389,8 +2619,12 @@
       <c r="E58" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <f>VLOOKUP(A58,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -2406,8 +2640,12 @@
       <c r="E59" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <f>VLOOKUP(A59,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -2423,8 +2661,12 @@
       <c r="E60" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <f>VLOOKUP(A60,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -2440,8 +2682,12 @@
       <c r="E61" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <f>VLOOKUP(A61,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -2457,8 +2703,12 @@
       <c r="E62" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <f>VLOOKUP(A62,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -2474,8 +2724,12 @@
       <c r="E63" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <f>VLOOKUP(A63,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -2491,8 +2745,12 @@
       <c r="E64" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <f>VLOOKUP(A64,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -2508,8 +2766,12 @@
       <c r="E65" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <f>VLOOKUP(A65,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -2525,8 +2787,12 @@
       <c r="E66" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <f>VLOOKUP(A66,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -2542,8 +2808,12 @@
       <c r="E67" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <f>VLOOKUP(A67,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -2559,8 +2829,12 @@
       <c r="E68" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <f>VLOOKUP(A68,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -2576,8 +2850,12 @@
       <c r="E69" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <f>VLOOKUP(A69,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2593,8 +2871,12 @@
       <c r="E70" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <f>VLOOKUP(A70,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -2610,8 +2892,12 @@
       <c r="E71" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <f>VLOOKUP(A71,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -2627,8 +2913,12 @@
       <c r="E72" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <f>VLOOKUP(A72,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -2644,8 +2934,12 @@
       <c r="E73" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <f>VLOOKUP(A73,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -2661,8 +2955,12 @@
       <c r="E74" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <f>VLOOKUP(A74,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -2678,8 +2976,12 @@
       <c r="E75" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <f>VLOOKUP(A75,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -2695,8 +2997,12 @@
       <c r="E76" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <f>VLOOKUP(A76,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -2712,8 +3018,12 @@
       <c r="E77" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <f>VLOOKUP(A77,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -2729,8 +3039,12 @@
       <c r="E78" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <f>VLOOKUP(A78,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -2746,8 +3060,12 @@
       <c r="E79" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <f>VLOOKUP(A79,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -2763,8 +3081,12 @@
       <c r="E80" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <f>VLOOKUP(A80,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -2780,8 +3102,12 @@
       <c r="E81" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <f>VLOOKUP(A81,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -2797,8 +3123,12 @@
       <c r="E82" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <f>VLOOKUP(A82,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -2814,8 +3144,12 @@
       <c r="E83" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <f>VLOOKUP(A83,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -2831,8 +3165,12 @@
       <c r="E84" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <f>VLOOKUP(A84,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -2848,8 +3186,12 @@
       <c r="E85" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <f>VLOOKUP(A85,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -2865,8 +3207,12 @@
       <c r="E86" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <f>VLOOKUP(A86,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -2882,8 +3228,12 @@
       <c r="E87" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <f>VLOOKUP(A87,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -2899,8 +3249,12 @@
       <c r="E88" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <f>VLOOKUP(A88,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>20</v>
       </c>
@@ -2916,8 +3270,12 @@
       <c r="E89" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <f>VLOOKUP(A89,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -2933,8 +3291,12 @@
       <c r="E90" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <f>VLOOKUP(A90,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>20</v>
       </c>
@@ -2950,8 +3312,12 @@
       <c r="E91" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <f>VLOOKUP(A91,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -2967,8 +3333,12 @@
       <c r="E92" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <f>VLOOKUP(A92,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -2984,8 +3354,12 @@
       <c r="E93" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <f>VLOOKUP(A93,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -3001,8 +3375,12 @@
       <c r="E94" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <f>VLOOKUP(A94,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -3018,8 +3396,12 @@
       <c r="E95" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <f>VLOOKUP(A95,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -3035,8 +3417,12 @@
       <c r="E96" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <f>VLOOKUP(A96,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -3052,8 +3438,12 @@
       <c r="E97" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <f>VLOOKUP(A97,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -3069,8 +3459,12 @@
       <c r="E98" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <f>VLOOKUP(A98,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -3086,8 +3480,12 @@
       <c r="E99" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <f>VLOOKUP(A99,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -3103,8 +3501,12 @@
       <c r="E100" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <f>VLOOKUP(A100,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -3120,8 +3522,12 @@
       <c r="E101" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <f>VLOOKUP(A101,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -3137,8 +3543,12 @@
       <c r="E102" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <f>VLOOKUP(A102,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>20</v>
       </c>
@@ -3154,8 +3564,12 @@
       <c r="E103" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <f>VLOOKUP(A103,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -3171,8 +3585,12 @@
       <c r="E104" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <f>VLOOKUP(A104,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3188,8 +3606,12 @@
       <c r="E105" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <f>VLOOKUP(A105,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>17</v>
       </c>
@@ -3205,8 +3627,12 @@
       <c r="E106" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <f>VLOOKUP(A106,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3222,8 +3648,12 @@
       <c r="E107" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <f>VLOOKUP(A107,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>14</v>
       </c>
@@ -3239,8 +3669,12 @@
       <c r="E108" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <f>VLOOKUP(A108,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -3256,8 +3690,12 @@
       <c r="E109" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <f>VLOOKUP(A109,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3273,8 +3711,12 @@
       <c r="E110" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110">
+        <f>VLOOKUP(A110,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -3290,8 +3732,12 @@
       <c r="E111" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111">
+        <f>VLOOKUP(A111,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>19</v>
       </c>
@@ -3307,8 +3753,12 @@
       <c r="E112" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112">
+        <f>VLOOKUP(A112,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>10</v>
       </c>
@@ -3324,8 +3774,12 @@
       <c r="E113" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113">
+        <f>VLOOKUP(A113,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -3341,8 +3795,12 @@
       <c r="E114" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114">
+        <f>VLOOKUP(A114,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>14</v>
       </c>
@@ -3358,8 +3816,12 @@
       <c r="E115" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115">
+        <f>VLOOKUP(A115,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -3375,8 +3837,12 @@
       <c r="E116" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116">
+        <f>VLOOKUP(A116,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -3392,8 +3858,12 @@
       <c r="E117" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117">
+        <f>VLOOKUP(A117,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -3409,8 +3879,12 @@
       <c r="E118" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118">
+        <f>VLOOKUP(A118,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>20</v>
       </c>
@@ -3426,8 +3900,12 @@
       <c r="E119" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119">
+        <f>VLOOKUP(A119,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -3443,8 +3921,12 @@
       <c r="E120" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120">
+        <f>VLOOKUP(A120,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -3460,8 +3942,12 @@
       <c r="E121" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121">
+        <f>VLOOKUP(A121,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>17</v>
       </c>
@@ -3477,8 +3963,12 @@
       <c r="E122" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122">
+        <f>VLOOKUP(A122,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>10</v>
       </c>
@@ -3494,8 +3984,12 @@
       <c r="E123" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123">
+        <f>VLOOKUP(A123,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>20</v>
       </c>
@@ -3511,8 +4005,12 @@
       <c r="E124" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124">
+        <f>VLOOKUP(A124,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -3528,8 +4026,12 @@
       <c r="E125" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125">
+        <f>VLOOKUP(A125,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -3545,8 +4047,12 @@
       <c r="E126" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126">
+        <f>VLOOKUP(A126,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>20</v>
       </c>
@@ -3562,8 +4068,12 @@
       <c r="E127" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F127">
+        <f>VLOOKUP(A127,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -3579,8 +4089,12 @@
       <c r="E128" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128">
+        <f>VLOOKUP(A128,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>19</v>
       </c>
@@ -3596,8 +4110,12 @@
       <c r="E129" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129">
+        <f>VLOOKUP(A129,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>15</v>
       </c>
@@ -3613,8 +4131,12 @@
       <c r="E130" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130">
+        <f>VLOOKUP(A130,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>4</v>
       </c>
@@ -3630,8 +4152,12 @@
       <c r="E131" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131">
+        <f>VLOOKUP(A131,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>20</v>
       </c>
@@ -3647,8 +4173,12 @@
       <c r="E132" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132">
+        <f>VLOOKUP(A132,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -3664,8 +4194,12 @@
       <c r="E133" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133">
+        <f>VLOOKUP(A133,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>10</v>
       </c>
@@ -3681,8 +4215,12 @@
       <c r="E134" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134">
+        <f>VLOOKUP(A134,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>4</v>
       </c>
@@ -3698,8 +4236,12 @@
       <c r="E135" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135">
+        <f>VLOOKUP(A135,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>6</v>
       </c>
@@ -3715,8 +4257,12 @@
       <c r="E136" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136">
+        <f>VLOOKUP(A136,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>15</v>
       </c>
@@ -3732,8 +4278,12 @@
       <c r="E137" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137">
+        <f>VLOOKUP(A137,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -3749,8 +4299,12 @@
       <c r="E138" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138">
+        <f>VLOOKUP(A138,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -3766,8 +4320,12 @@
       <c r="E139" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F139">
+        <f>VLOOKUP(A139,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>14</v>
       </c>
@@ -3783,8 +4341,12 @@
       <c r="E140" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140">
+        <f>VLOOKUP(A140,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -3800,8 +4362,12 @@
       <c r="E141" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141">
+        <f>VLOOKUP(A141,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -3817,8 +4383,12 @@
       <c r="E142" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142">
+        <f>VLOOKUP(A142,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -3834,8 +4404,12 @@
       <c r="E143" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143">
+        <f>VLOOKUP(A143,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -3851,8 +4425,12 @@
       <c r="E144" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144">
+        <f>VLOOKUP(A144,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>6</v>
       </c>
@@ -3868,8 +4446,12 @@
       <c r="E145" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F145">
+        <f>VLOOKUP(A145,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>18</v>
       </c>
@@ -3885,8 +4467,12 @@
       <c r="E146" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F146">
+        <f>VLOOKUP(A146,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>6</v>
       </c>
@@ -3902,8 +4488,12 @@
       <c r="E147" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F147">
+        <f>VLOOKUP(A147,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -3919,8 +4509,12 @@
       <c r="E148" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F148">
+        <f>VLOOKUP(A148,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>18</v>
       </c>
@@ -3936,8 +4530,12 @@
       <c r="E149" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F149">
+        <f>VLOOKUP(A149,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>21</v>
       </c>
@@ -3953,8 +4551,12 @@
       <c r="E150" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F150">
+        <f>VLOOKUP(A150,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>8</v>
       </c>
@@ -3970,8 +4572,12 @@
       <c r="E151" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F151">
+        <f>VLOOKUP(A151,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -3987,8 +4593,12 @@
       <c r="E152" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F152">
+        <f>VLOOKUP(A152,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -4004,8 +4614,12 @@
       <c r="E153" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F153">
+        <f>VLOOKUP(A153,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>6</v>
       </c>
@@ -4021,8 +4635,12 @@
       <c r="E154" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F154">
+        <f>VLOOKUP(A154,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -4038,8 +4656,12 @@
       <c r="E155" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F155">
+        <f>VLOOKUP(A155,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>21</v>
       </c>
@@ -4055,8 +4677,12 @@
       <c r="E156" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F156">
+        <f>VLOOKUP(A156,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -4072,8 +4698,12 @@
       <c r="E157" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F157">
+        <f>VLOOKUP(A157,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>8</v>
       </c>
@@ -4089,8 +4719,12 @@
       <c r="E158" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F158">
+        <f>VLOOKUP(A158,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>14</v>
       </c>
@@ -4106,8 +4740,12 @@
       <c r="E159" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F159">
+        <f>VLOOKUP(A159,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>18</v>
       </c>
@@ -4123,8 +4761,12 @@
       <c r="E160" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F160">
+        <f>VLOOKUP(A160,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>19</v>
       </c>
@@ -4140,8 +4782,12 @@
       <c r="E161" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F161">
+        <f>VLOOKUP(A161,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>18</v>
       </c>
@@ -4157,8 +4803,12 @@
       <c r="E162" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F162">
+        <f>VLOOKUP(A162,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>17</v>
       </c>
@@ -4174,8 +4824,12 @@
       <c r="E163" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F163">
+        <f>VLOOKUP(A163,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>21</v>
       </c>
@@ -4191,8 +4845,12 @@
       <c r="E164" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F164">
+        <f>VLOOKUP(A164,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>8</v>
       </c>
@@ -4208,8 +4866,12 @@
       <c r="E165" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F165">
+        <f>VLOOKUP(A165,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>21</v>
       </c>
@@ -4225,8 +4887,12 @@
       <c r="E166" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F166">
+        <f>VLOOKUP(A166,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>14</v>
       </c>
@@ -4242,8 +4908,12 @@
       <c r="E167" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F167">
+        <f>VLOOKUP(A167,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>15</v>
       </c>
@@ -4259,8 +4929,12 @@
       <c r="E168" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F168">
+        <f>VLOOKUP(A168,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>21</v>
       </c>
@@ -4276,8 +4950,12 @@
       <c r="E169" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F169">
+        <f>VLOOKUP(A169,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>19</v>
       </c>
@@ -4293,8 +4971,12 @@
       <c r="E170" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F170">
+        <f>VLOOKUP(A170,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>15</v>
       </c>
@@ -4310,8 +4992,12 @@
       <c r="E171" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F171">
+        <f>VLOOKUP(A171,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>18</v>
       </c>
@@ -4327,8 +5013,12 @@
       <c r="E172" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F172">
+        <f>VLOOKUP(A172,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>17</v>
       </c>
@@ -4344,8 +5034,12 @@
       <c r="E173" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F173">
+        <f>VLOOKUP(A173,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>4</v>
       </c>
@@ -4361,8 +5055,12 @@
       <c r="E174" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174">
+        <f>VLOOKUP(A174,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>21</v>
       </c>
@@ -4378,8 +5076,12 @@
       <c r="E175" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175">
+        <f>VLOOKUP(A175,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>21</v>
       </c>
@@ -4395,8 +5097,12 @@
       <c r="E176" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F176">
+        <f>VLOOKUP(A176,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>21</v>
       </c>
@@ -4412,8 +5118,12 @@
       <c r="E177" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F177">
+        <f>VLOOKUP(A177,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>4</v>
       </c>
@@ -4429,8 +5139,12 @@
       <c r="E178" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F178">
+        <f>VLOOKUP(A178,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>21</v>
       </c>
@@ -4446,8 +5160,12 @@
       <c r="E179" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F179">
+        <f>VLOOKUP(A179,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>19</v>
       </c>
@@ -4463,8 +5181,12 @@
       <c r="E180" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F180">
+        <f>VLOOKUP(A180,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>9</v>
       </c>
@@ -4480,8 +5202,12 @@
       <c r="E181" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F181">
+        <f>VLOOKUP(A181,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>4</v>
       </c>
@@ -4497,8 +5223,12 @@
       <c r="E182" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F182">
+        <f>VLOOKUP(A182,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>8</v>
       </c>
@@ -4514,8 +5244,12 @@
       <c r="E183" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F183">
+        <f>VLOOKUP(A183,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>21</v>
       </c>
@@ -4531,8 +5265,12 @@
       <c r="E184" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F184">
+        <f>VLOOKUP(A184,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -4548,8 +5286,12 @@
       <c r="E185" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F185">
+        <f>VLOOKUP(A185,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>14</v>
       </c>
@@ -4565,8 +5307,12 @@
       <c r="E186" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F186">
+        <f>VLOOKUP(A186,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>17</v>
       </c>
@@ -4582,8 +5328,12 @@
       <c r="E187" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F187">
+        <f>VLOOKUP(A187,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>10</v>
       </c>
@@ -4599,8 +5349,12 @@
       <c r="E188" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F188">
+        <f>VLOOKUP(A188,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>9</v>
       </c>
@@ -4616,8 +5370,12 @@
       <c r="E189" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F189">
+        <f>VLOOKUP(A189,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>21</v>
       </c>
@@ -4633,8 +5391,12 @@
       <c r="E190" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F190">
+        <f>VLOOKUP(A190,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>19</v>
       </c>
@@ -4650,8 +5412,12 @@
       <c r="E191" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F191">
+        <f>VLOOKUP(A191,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>9</v>
       </c>
@@ -4667,8 +5433,12 @@
       <c r="E192" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F192">
+        <f>VLOOKUP(A192,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>10</v>
       </c>
@@ -4684,8 +5454,12 @@
       <c r="E193" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F193">
+        <f>VLOOKUP(A193,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>8</v>
       </c>
@@ -4701,8 +5475,12 @@
       <c r="E194" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F194">
+        <f>VLOOKUP(A194,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>4</v>
       </c>
@@ -4718,8 +5496,12 @@
       <c r="E195" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F195">
+        <f>VLOOKUP(A195,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>9</v>
       </c>
@@ -4735,8 +5517,12 @@
       <c r="E196" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F196">
+        <f>VLOOKUP(A196,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>21</v>
       </c>
@@ -4752,8 +5538,12 @@
       <c r="E197" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F197">
+        <f>VLOOKUP(A197,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>15</v>
       </c>
@@ -4769,8 +5559,12 @@
       <c r="E198" s="6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F198">
+        <f>VLOOKUP(A198,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>10</v>
       </c>
@@ -4786,8 +5580,12 @@
       <c r="E199" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F199">
+        <f>VLOOKUP(A199,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>21</v>
       </c>
@@ -4803,13 +5601,17 @@
       <c r="E200" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F200">
+        <f>VLOOKUP(A200,Calories!$A$1:$B$15,2,FALSE)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C202" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C203" s="4">
         <f>AVERAGE(C2:C200)</f>
         <v>2.829145728643216</v>
@@ -4834,7 +5636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -4845,7 +5647,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4962,7 +5764,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <f>MATCH("Hamburger", A2:A15, 0)</f>
@@ -4971,7 +5773,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <f>INDEX(A1:B15,3, 2)</f>
@@ -4980,7 +5782,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" t="str">
         <f ca="1">OFFSET(A1,3,0)</f>
@@ -4989,7 +5791,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <f>SMALL(B2:B15, 3)</f>

</xml_diff>

<commit_message>
Get revenue by item through  pivot table
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -2,23 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathaniel/Desktop/side/data-smart/chapter-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Basketball Game Sales" sheetId="1" r:id="rId1"/>
-    <sheet name="Calories" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Revenue by Item" sheetId="4" r:id="rId2"/>
+    <sheet name="Basketball Game Sales" sheetId="1" r:id="rId3"/>
+    <sheet name="Calories" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Basketball Game Sales'!$A$1:$F$203</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Basketball Game Sales'!$A$1:$F$203</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="34">
   <si>
     <t>Item</t>
   </si>
@@ -122,6 +127,18 @@
   <si>
     <t>Small</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Price</t>
+  </si>
 </sst>
 </file>
 
@@ -131,7 +148,7 @@
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,16 +163,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor theme="9" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -183,13 +221,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color theme="9" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -203,6 +270,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" pivotButton="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1139,6 +1221,1940 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="42498.70837453704" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="203">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:F1048576" sheet="Basketball Game Sales"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Item" numFmtId="0">
+      <sharedItems containsBlank="1" count="15">
+        <s v="Beer"/>
+        <s v="Hamburger"/>
+        <s v="Popcorn"/>
+        <s v="Pizza"/>
+        <s v="Bottled Water"/>
+        <s v="Hot Dog"/>
+        <s v="Chocolate Dipped Cone"/>
+        <s v="Soda"/>
+        <s v="Chocolate Bar"/>
+        <s v="Licorice Rope"/>
+        <s v="Nachos"/>
+        <s v="Gummy Bears"/>
+        <s v="Ice Cream Sandwich"/>
+        <s v="Popsicle"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems containsBlank="1" count="5">
+        <s v="Beverages"/>
+        <s v="Hot Food"/>
+        <s v="Frozen Treats"/>
+        <s v="Candy"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Price" numFmtId="0">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="1.5" maxValue="5" count="9">
+        <n v="4"/>
+        <n v="3"/>
+        <n v="5"/>
+        <n v="2"/>
+        <n v="1.5"/>
+        <n v="2.5"/>
+        <m/>
+        <s v="AVERAGE"/>
+        <n v="2.829145728643216"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Profit" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="0.83333333333333337"/>
+    </cacheField>
+    <cacheField name="Actual Profit" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="4"/>
+    </cacheField>
+    <cacheField name="Calories" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="560"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="203">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="240"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.66666666666666663"/>
+    <n v="2"/>
+    <n v="320"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.5"/>
+    <n v="1.5"/>
+    <n v="560"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="1"/>
+    <n v="265"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="0.8"/>
+    <n v="2"/>
+    <n v="120"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="280"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.5"/>
+    <n v="1"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0.8"/>
+    <n v="4"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="2"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.25"/>
+    <n v="0.5"/>
+    <n v="480"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0.75"/>
+    <n v="1.5"/>
+    <n v="255"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0.83333333333333337"/>
+    <n v="2.5"/>
+    <n v="150"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="4"/>
+    <x v="6"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="4"/>
+    <x v="7"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="4"/>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="14"/>
+    <x v="4"/>
+    <x v="6"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="12"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="10">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Price" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="16">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="12"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="14"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="10">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Price" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1402,10 +3418,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="14">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="14">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="14">
+        <v>2.829145728643216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="14">
+        <v>565.8291457286432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="16">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2.829145728643216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="17">
+        <v>565.8291457286432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5636,7 +7962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>

</xml_diff>

<commit_message>
Calculate total calorie count sold by category
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -14,15 +14,17 @@
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
     <sheet name="Revenue by Item" sheetId="4" r:id="rId2"/>
-    <sheet name="Basketball Game Sales" sheetId="1" r:id="rId3"/>
-    <sheet name="Calories" sheetId="2" r:id="rId4"/>
+    <sheet name="Total Calorie Sold by Category" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
+    <sheet name="Basketball Game Sales" sheetId="1" r:id="rId5"/>
+    <sheet name="Calories" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Basketball Game Sales'!$A$1:$F$203</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Basketball Game Sales'!$A$1:$F$203</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="35">
   <si>
     <t>Item</t>
   </si>
@@ -139,6 +141,9 @@
   <si>
     <t>Sum of Price</t>
   </si>
+  <si>
+    <t>Sum of Calories</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +153,7 @@
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,37 +168,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor theme="9" tint="-0.249977111117893"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -221,42 +205,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color theme="9" tint="-0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -274,17 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" pivotButton="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1275,7 +1220,22 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="4"/>
     </cacheField>
     <cacheField name="Calories" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="560"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="560" count="14">
+        <n v="200"/>
+        <n v="320"/>
+        <n v="500"/>
+        <n v="480"/>
+        <n v="0"/>
+        <n v="265"/>
+        <n v="300"/>
+        <n v="120"/>
+        <n v="255"/>
+        <n v="280"/>
+        <n v="560"/>
+        <n v="240"/>
+        <n v="150"/>
+        <m/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1294,7 +1254,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -1302,7 +1262,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="2"/>
@@ -1310,7 +1270,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="3"/>
@@ -1318,7 +1278,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="4"/>
@@ -1326,7 +1286,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="5"/>
@@ -1334,7 +1294,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="6"/>
@@ -1342,7 +1302,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="7"/>
@@ -1350,7 +1310,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="8"/>
@@ -1358,7 +1318,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="1"/>
@@ -1366,7 +1326,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -1374,7 +1334,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -1382,7 +1342,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="9"/>
@@ -1390,7 +1350,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="6"/>
@@ -1398,7 +1358,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="10"/>
@@ -1406,7 +1366,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="3"/>
@@ -1414,7 +1374,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
@@ -1422,7 +1382,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="7"/>
@@ -1430,7 +1390,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="0"/>
@@ -1438,7 +1398,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -1446,7 +1406,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="11"/>
@@ -1454,7 +1414,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="2"/>
@@ -1462,7 +1422,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="1"/>
@@ -1470,7 +1430,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="10"/>
@@ -1478,15 +1438,15 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
-  </r>
-  <r>
     <x v="10"/>
+  </r>
+  <r>
+    <x v="10"/>
     <x v="1"/>
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="6"/>
@@ -1494,7 +1454,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="8"/>
@@ -1502,7 +1462,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="1"/>
@@ -1510,7 +1470,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -1518,7 +1478,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -1526,7 +1486,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="7"/>
@@ -1534,7 +1494,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="11"/>
@@ -1542,7 +1502,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="6"/>
@@ -1550,7 +1510,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="9"/>
@@ -1558,7 +1518,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="10"/>
@@ -1566,7 +1526,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="4"/>
@@ -1574,7 +1534,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="4"/>
@@ -1582,7 +1542,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="2"/>
@@ -1590,7 +1550,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="8"/>
@@ -1598,7 +1558,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="6"/>
@@ -1606,7 +1566,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="9"/>
@@ -1614,7 +1574,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="0"/>
@@ -1622,7 +1582,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -1630,7 +1590,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="8"/>
@@ -1638,7 +1598,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="3"/>
@@ -1646,7 +1606,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
@@ -1654,7 +1614,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="6"/>
@@ -1662,7 +1622,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="9"/>
@@ -1670,7 +1630,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="10"/>
@@ -1678,7 +1638,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="2"/>
@@ -1686,7 +1646,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="8"/>
@@ -1694,7 +1654,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="5"/>
@@ -1702,7 +1662,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="2"/>
@@ -1710,7 +1670,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -1718,7 +1678,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -1726,7 +1686,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="11"/>
@@ -1734,7 +1694,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="9"/>
@@ -1742,7 +1702,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="0"/>
@@ -1750,7 +1710,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="9"/>
@@ -1758,7 +1718,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="0"/>
@@ -1766,7 +1726,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="7"/>
@@ -1774,7 +1734,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="5"/>
@@ -1782,7 +1742,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="3"/>
@@ -1790,7 +1750,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="7"/>
@@ -1798,7 +1758,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="11"/>
@@ -1806,7 +1766,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="6"/>
@@ -1814,7 +1774,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="7"/>
@@ -1822,7 +1782,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="8"/>
@@ -1830,7 +1790,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="0"/>
@@ -1838,7 +1798,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -1846,7 +1806,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
@@ -1854,7 +1814,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="10"/>
@@ -1862,23 +1822,23 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
-  </r>
-  <r>
     <x v="10"/>
+  </r>
+  <r>
+    <x v="10"/>
     <x v="1"/>
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
-  </r>
-  <r>
     <x v="10"/>
+  </r>
+  <r>
+    <x v="10"/>
     <x v="1"/>
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="11"/>
@@ -1886,7 +1846,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="5"/>
@@ -1894,7 +1854,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="3"/>
@@ -1902,7 +1862,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="4"/>
@@ -1910,7 +1870,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="1"/>
@@ -1918,7 +1878,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="6"/>
@@ -1926,7 +1886,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="2"/>
@@ -1934,7 +1894,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="5"/>
@@ -1942,7 +1902,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="12"/>
@@ -1950,7 +1910,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="8"/>
@@ -1958,7 +1918,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="9"/>
@@ -1966,7 +1926,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="0"/>
@@ -1974,7 +1934,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -1982,7 +1942,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="12"/>
@@ -1990,7 +1950,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="5"/>
@@ -1998,7 +1958,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="12"/>
@@ -2006,7 +1966,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="7"/>
@@ -2014,7 +1974,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="8"/>
@@ -2022,7 +1982,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="11"/>
@@ -2030,7 +1990,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="3"/>
@@ -2038,7 +1998,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="5"/>
@@ -2046,7 +2006,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="11"/>
@@ -2054,7 +2014,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="12"/>
@@ -2062,7 +2022,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="9"/>
@@ -2070,7 +2030,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="0"/>
@@ -2078,7 +2038,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2086,7 +2046,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
@@ -2094,7 +2054,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="12"/>
@@ -2102,15 +2062,15 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
-  </r>
-  <r>
     <x v="11"/>
+  </r>
+  <r>
+    <x v="11"/>
     <x v="3"/>
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="1"/>
@@ -2118,7 +2078,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="9"/>
@@ -2126,7 +2086,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="1"/>
@@ -2134,7 +2094,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="7"/>
@@ -2142,7 +2102,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="4"/>
@@ -2150,7 +2110,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="1"/>
@@ -2158,7 +2118,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="12"/>
@@ -2166,15 +2126,15 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
-  </r>
-  <r>
     <x v="11"/>
+  </r>
+  <r>
+    <x v="11"/>
     <x v="3"/>
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="4"/>
@@ -2182,7 +2142,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="5"/>
@@ -2190,7 +2150,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="7"/>
@@ -2198,7 +2158,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="3"/>
@@ -2206,7 +2166,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="2"/>
@@ -2214,7 +2174,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="2"/>
@@ -2222,7 +2182,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="12"/>
@@ -2230,7 +2190,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="2"/>
@@ -2238,7 +2198,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="4"/>
@@ -2246,7 +2206,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="9"/>
@@ -2254,7 +2214,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="4"/>
@@ -2262,7 +2222,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="12"/>
@@ -2270,7 +2230,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="3"/>
@@ -2278,7 +2238,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="3"/>
@@ -2286,7 +2246,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="12"/>
@@ -2294,7 +2254,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="3"/>
@@ -2302,7 +2262,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="11"/>
@@ -2310,7 +2270,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="8"/>
@@ -2318,7 +2278,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="0"/>
@@ -2326,7 +2286,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="12"/>
@@ -2334,7 +2294,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="240"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="10"/>
@@ -2342,7 +2302,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="4"/>
@@ -2350,7 +2310,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="0"/>
@@ -2358,7 +2318,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2366,7 +2326,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="8"/>
@@ -2374,7 +2334,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="2"/>
@@ -2382,7 +2342,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="1"/>
@@ -2390,7 +2350,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="7"/>
@@ -2398,7 +2358,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="3"/>
@@ -2406,7 +2366,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="5"/>
@@ -2414,7 +2374,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="5"/>
@@ -2422,7 +2382,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="10"/>
@@ -2430,7 +2390,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="1"/>
@@ -2438,7 +2398,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="10"/>
@@ -2446,7 +2406,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="1"/>
@@ -2454,7 +2414,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="5"/>
@@ -2462,7 +2422,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="10"/>
@@ -2470,7 +2430,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="13"/>
@@ -2478,7 +2438,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="2"/>
@@ -2486,7 +2446,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="2"/>
@@ -2494,7 +2454,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="4"/>
@@ -2502,7 +2462,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="1"/>
@@ -2510,7 +2470,7 @@
     <x v="1"/>
     <n v="0.66666666666666663"/>
     <n v="2"/>
-    <n v="320"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="3"/>
@@ -2518,7 +2478,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="13"/>
@@ -2526,7 +2486,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="3"/>
@@ -2534,7 +2494,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="2"/>
@@ -2542,7 +2502,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="7"/>
@@ -2550,7 +2510,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="10"/>
@@ -2558,7 +2518,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="11"/>
@@ -2566,7 +2526,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="10"/>
@@ -2574,7 +2534,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="9"/>
@@ -2582,7 +2542,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="13"/>
@@ -2590,7 +2550,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="2"/>
@@ -2598,7 +2558,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="13"/>
@@ -2606,7 +2566,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="7"/>
@@ -2614,7 +2574,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="8"/>
@@ -2622,7 +2582,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="13"/>
@@ -2630,7 +2590,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="11"/>
@@ -2638,7 +2598,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="8"/>
@@ -2646,7 +2606,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="10"/>
@@ -2654,7 +2614,7 @@
     <x v="1"/>
     <n v="0.5"/>
     <n v="1.5"/>
-    <n v="560"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="9"/>
@@ -2662,7 +2622,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="0"/>
@@ -2670,7 +2630,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="13"/>
@@ -2678,7 +2638,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="13"/>
@@ -2686,7 +2646,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="13"/>
@@ -2694,7 +2654,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="0"/>
@@ -2702,7 +2662,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="13"/>
@@ -2710,7 +2670,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="11"/>
@@ -2718,7 +2678,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="3"/>
@@ -2726,7 +2686,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
@@ -2734,7 +2694,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2742,7 +2702,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="13"/>
@@ -2750,7 +2710,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="5"/>
@@ -2758,7 +2718,7 @@
     <x v="4"/>
     <n v="0.66666666666666663"/>
     <n v="1"/>
-    <n v="265"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="7"/>
@@ -2766,7 +2726,7 @@
     <x v="5"/>
     <n v="0.8"/>
     <n v="2"/>
-    <n v="120"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="9"/>
@@ -2774,7 +2734,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="280"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="4"/>
@@ -2782,7 +2742,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="3"/>
@@ -2790,7 +2750,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="13"/>
@@ -2798,7 +2758,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="11"/>
@@ -2806,7 +2766,7 @@
     <x v="3"/>
     <n v="0.5"/>
     <n v="1"/>
-    <n v="300"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="3"/>
@@ -2814,7 +2774,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="4"/>
@@ -2822,7 +2782,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="2"/>
@@ -2830,7 +2790,7 @@
     <x v="2"/>
     <n v="0.8"/>
     <n v="4"/>
-    <n v="500"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
@@ -2838,7 +2798,7 @@
     <x v="0"/>
     <n v="0.5"/>
     <n v="2"/>
-    <n v="200"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2846,7 +2806,7 @@
     <x v="3"/>
     <n v="0.25"/>
     <n v="0.5"/>
-    <n v="480"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="13"/>
@@ -2854,7 +2814,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="8"/>
@@ -2862,7 +2822,7 @@
     <x v="3"/>
     <n v="0.75"/>
     <n v="1.5"/>
-    <n v="255"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="4"/>
@@ -2870,7 +2830,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="0"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="13"/>
@@ -2878,7 +2838,7 @@
     <x v="1"/>
     <n v="0.83333333333333337"/>
     <n v="2.5"/>
-    <n v="150"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="14"/>
@@ -2886,7 +2846,7 @@
     <x v="6"/>
     <m/>
     <m/>
-    <m/>
+    <x v="13"/>
   </r>
   <r>
     <x v="14"/>
@@ -2894,7 +2854,7 @@
     <x v="7"/>
     <m/>
     <m/>
-    <m/>
+    <x v="13"/>
   </r>
   <r>
     <x v="14"/>
@@ -2902,7 +2862,7 @@
     <x v="8"/>
     <m/>
     <m/>
-    <m/>
+    <x v="13"/>
   </r>
   <r>
     <x v="14"/>
@@ -2910,13 +2870,13 @@
     <x v="6"/>
     <m/>
     <m/>
-    <m/>
+    <x v="13"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -3036,30 +2996,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="16">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="6"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="13"/>
-        <item x="7"/>
-        <item x="14"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
       <items count="6">
         <item x="0"/>
         <item x="3"/>
@@ -3069,28 +3010,33 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0">
-      <items count="10">
+      <items count="15">
         <item x="4"/>
+        <item x="7"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="1"/>
         <item x="3"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="0"/>
         <item x="2"/>
-        <item x="7"/>
-        <item x="6"/>
+        <item x="10"/>
+        <item x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="0"/>
+    <field x="1"/>
   </rowFields>
-  <rowItems count="16">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -3106,36 +3052,6 @@
     <i>
       <x v="4"/>
     </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -3144,7 +3060,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Price" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Calories" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3446,7 +3362,7 @@
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>80</v>
       </c>
     </row>
@@ -3454,7 +3370,7 @@
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>39</v>
       </c>
     </row>
@@ -3462,7 +3378,7 @@
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>26</v>
       </c>
     </row>
@@ -3470,7 +3386,7 @@
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>33</v>
       </c>
     </row>
@@ -3478,7 +3394,7 @@
       <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>28</v>
       </c>
     </row>
@@ -3486,7 +3402,7 @@
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>48</v>
       </c>
     </row>
@@ -3494,7 +3410,7 @@
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>22.5</v>
       </c>
     </row>
@@ -3502,7 +3418,7 @@
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>30</v>
       </c>
     </row>
@@ -3510,7 +3426,7 @@
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>26</v>
       </c>
     </row>
@@ -3518,7 +3434,7 @@
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>45</v>
       </c>
     </row>
@@ -3526,7 +3442,7 @@
       <c r="A14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>34</v>
       </c>
     </row>
@@ -3534,7 +3450,7 @@
       <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="11">
         <v>80</v>
       </c>
     </row>
@@ -3542,7 +3458,7 @@
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="11">
         <v>39</v>
       </c>
     </row>
@@ -3550,7 +3466,7 @@
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="11">
         <v>32.5</v>
       </c>
     </row>
@@ -3558,7 +3474,7 @@
       <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="11">
         <v>2.829145728643216</v>
       </c>
     </row>
@@ -3566,7 +3482,7 @@
       <c r="A19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="11">
         <v>565.8291457286432</v>
       </c>
     </row>
@@ -3580,144 +3496,144 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8">
         <v>22.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15">
         <v>32.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16">
         <v>2.829145728643216</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17">
         <v>565.8291457286432</v>
       </c>
     </row>
@@ -3727,6 +3643,142 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5560</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>11155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>7650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>33655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>58020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11">
+        <v>5560</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11">
+        <v>11155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="11">
+        <v>7650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11">
+        <v>33655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="11">
+        <v>58020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F203"/>
   <sheetViews>
@@ -7962,7 +8014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>

</xml_diff>

<commit_message>
Calculate cut for coach
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="38">
   <si>
     <t>Item</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>Total Cut for Coach</t>
+  </si>
+  <si>
+    <t>Sum Product</t>
   </si>
 </sst>
 </file>
@@ -3497,31 +3503,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f t="array" ref="C2">SUMPRODUCT(B2:B15,TRANSPOSE('Fee Schedule'!B2:O2))</f>
+        <v>57.6</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3529,7 +3548,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3537,7 +3556,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3545,7 +3564,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -3553,7 +3572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3561,7 +3580,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3569,7 +3588,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -3577,7 +3596,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3585,7 +3604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3593,7 +3612,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3601,7 +3620,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3609,7 +3628,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3617,7 +3636,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3625,7 +3644,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3650,7 +3669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Use solver to find minimum number of products needed to reach 2400 calories
</commit_message>
<xml_diff>
--- a/exercise-01.xlsx
+++ b/exercise-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25740" windowHeight="17460" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="17460" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basketball Game Sales" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,42 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Basketball Game Sales'!$A$1:$F$203</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">'Calories-Solver'!$C$2:$C$15</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">'Calories-Solver'!$C$17</definedName>
+    <definedName name="solver_lhs2" localSheetId="7" hidden="1">'Calories-Solver'!$C$2:$C$15</definedName>
+    <definedName name="solver_lin" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'Calories-Solver'!$C$16</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="7" hidden="1">4</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">2400</definedName>
+    <definedName name="solver_rhs2" localSheetId="7" hidden="1">integer</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -40,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="41">
   <si>
     <t>Item</t>
   </si>
@@ -154,6 +186,15 @@
   </si>
   <si>
     <t>Sum Product</t>
+  </si>
+  <si>
+    <t>How many?</t>
+  </si>
+  <si>
+    <t>Total Items</t>
+  </si>
+  <si>
+    <t>Total Calories</t>
   </si>
 </sst>
 </file>
@@ -272,7 +313,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -445,11 +485,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2092002624"/>
-        <c:axId val="-2089652448"/>
+        <c:axId val="2126374288"/>
+        <c:axId val="2126377552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2092002624"/>
+        <c:axId val="2126374288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089652448"/>
+        <c:crossAx val="2126377552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -500,7 +540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2089652448"/>
+        <c:axId val="2126377552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,7 +590,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092002624"/>
+        <c:crossAx val="2126374288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2887,7 +2927,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -3007,7 +3047,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -8321,135 +8361,199 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B4">
         <v>255</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B5">
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B6">
         <v>300</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>320</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B8">
         <v>265</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B9">
         <v>240</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B10">
         <v>280</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B11">
         <v>560</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B12">
         <v>480</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <v>500</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B14">
         <v>150</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <v>120</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C2:C15)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <f>SUMPRODUCT(B2:B15,C2:C15)</f>
+        <v>2400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>